<commit_message>
Cambios para taller 8
</commit_message>
<xml_diff>
--- a/Bases de datos/trm2020.xlsx
+++ b/Bases de datos/trm2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arias\Documents\Jorge trabajo\UExternado\Economia\ux ECO econometria R\ux economR 2021 1\talleres\taller07 ts arima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87557C98-3919-4862-BEEC-8D248E3C24E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40128B5-EDB4-4CA6-A8F4-7B7A7AED4333}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B6B407D-C706-478A-B9B7-AAC953FAB9F0}"/>
+    <workbookView xWindow="28335" yWindow="405" windowWidth="17550" windowHeight="14085" xr2:uid="{4B6B407D-C706-478A-B9B7-AAC953FAB9F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -485,11 +485,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A105433-E580-40A5-BB27-5897456A869F}">
-  <dimension ref="A1:B5918"/>
+  <dimension ref="A1:B5956"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -47837,6 +47835,310 @@
         <v>3575.3</v>
       </c>
     </row>
+    <row r="5919" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5919" s="4">
+        <v>44270</v>
+      </c>
+      <c r="B5919" s="6">
+        <v>3575.3</v>
+      </c>
+    </row>
+    <row r="5920" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5920" s="3">
+        <v>44271</v>
+      </c>
+      <c r="B5920" s="5">
+        <v>3575.63</v>
+      </c>
+    </row>
+    <row r="5921" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5921" s="4">
+        <v>44272</v>
+      </c>
+      <c r="B5921" s="6">
+        <v>3553.51</v>
+      </c>
+    </row>
+    <row r="5922" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5922" s="3">
+        <v>44273</v>
+      </c>
+      <c r="B5922" s="5">
+        <v>3578.02</v>
+      </c>
+    </row>
+    <row r="5923" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5923" s="4">
+        <v>44274</v>
+      </c>
+      <c r="B5923" s="6">
+        <v>3569.45</v>
+      </c>
+    </row>
+    <row r="5924" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5924" s="3">
+        <v>44275</v>
+      </c>
+      <c r="B5924" s="5">
+        <v>3553.34</v>
+      </c>
+    </row>
+    <row r="5925" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5925" s="4">
+        <v>44276</v>
+      </c>
+      <c r="B5925" s="6">
+        <v>3553.34</v>
+      </c>
+    </row>
+    <row r="5926" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5926" s="3">
+        <v>44277</v>
+      </c>
+      <c r="B5926" s="5">
+        <v>3553.34</v>
+      </c>
+    </row>
+    <row r="5927" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5927" s="4">
+        <v>44278</v>
+      </c>
+      <c r="B5927" s="6">
+        <v>3553.34</v>
+      </c>
+    </row>
+    <row r="5928" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5928" s="3">
+        <v>44279</v>
+      </c>
+      <c r="B5928" s="5">
+        <v>3589.82</v>
+      </c>
+    </row>
+    <row r="5929" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5929" s="4">
+        <v>44280</v>
+      </c>
+      <c r="B5929" s="6">
+        <v>3635.12</v>
+      </c>
+    </row>
+    <row r="5930" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5930" s="3">
+        <v>44281</v>
+      </c>
+      <c r="B5930" s="5">
+        <v>3658.22</v>
+      </c>
+    </row>
+    <row r="5931" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5931" s="4">
+        <v>44282</v>
+      </c>
+      <c r="B5931" s="6">
+        <v>3665.41</v>
+      </c>
+    </row>
+    <row r="5932" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5932" s="3">
+        <v>44283</v>
+      </c>
+      <c r="B5932" s="5">
+        <v>3665.41</v>
+      </c>
+    </row>
+    <row r="5933" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5933" s="4">
+        <v>44284</v>
+      </c>
+      <c r="B5933" s="6">
+        <v>3665.41</v>
+      </c>
+    </row>
+    <row r="5934" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5934" s="3">
+        <v>44285</v>
+      </c>
+      <c r="B5934" s="5">
+        <v>3705.85</v>
+      </c>
+    </row>
+    <row r="5935" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5935" s="4">
+        <v>44286</v>
+      </c>
+      <c r="B5935" s="6">
+        <v>3736.91</v>
+      </c>
+    </row>
+    <row r="5936" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5936" s="3">
+        <v>44287</v>
+      </c>
+      <c r="B5936" s="5">
+        <v>3678.62</v>
+      </c>
+    </row>
+    <row r="5937" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5937" s="4">
+        <v>44288</v>
+      </c>
+      <c r="B5937" s="6">
+        <v>3678.62</v>
+      </c>
+    </row>
+    <row r="5938" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5938" s="3">
+        <v>44289</v>
+      </c>
+      <c r="B5938" s="5">
+        <v>3678.62</v>
+      </c>
+    </row>
+    <row r="5939" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5939" s="4">
+        <v>44290</v>
+      </c>
+      <c r="B5939" s="6">
+        <v>3678.62</v>
+      </c>
+    </row>
+    <row r="5940" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5940" s="3">
+        <v>44291</v>
+      </c>
+      <c r="B5940" s="5">
+        <v>3678.62</v>
+      </c>
+    </row>
+    <row r="5941" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5941" s="4">
+        <v>44292</v>
+      </c>
+      <c r="B5941" s="6">
+        <v>3645.79</v>
+      </c>
+    </row>
+    <row r="5942" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5942" s="3">
+        <v>44293</v>
+      </c>
+      <c r="B5942" s="5">
+        <v>3645.14</v>
+      </c>
+    </row>
+    <row r="5943" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5943" s="4">
+        <v>44294</v>
+      </c>
+      <c r="B5943" s="6">
+        <v>3639.62</v>
+      </c>
+    </row>
+    <row r="5944" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5944" s="3">
+        <v>44295</v>
+      </c>
+      <c r="B5944" s="5">
+        <v>3634.07</v>
+      </c>
+    </row>
+    <row r="5945" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5945" s="4">
+        <v>44296</v>
+      </c>
+      <c r="B5945" s="6">
+        <v>3650.23</v>
+      </c>
+    </row>
+    <row r="5946" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5946" s="3">
+        <v>44297</v>
+      </c>
+      <c r="B5946" s="5">
+        <v>3650.23</v>
+      </c>
+    </row>
+    <row r="5947" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5947" s="4">
+        <v>44298</v>
+      </c>
+      <c r="B5947" s="6">
+        <v>3650.23</v>
+      </c>
+    </row>
+    <row r="5948" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5948" s="3">
+        <v>44299</v>
+      </c>
+      <c r="B5948" s="5">
+        <v>3653.57</v>
+      </c>
+    </row>
+    <row r="5949" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5949" s="4">
+        <v>44300</v>
+      </c>
+      <c r="B5949" s="6">
+        <v>3666.17</v>
+      </c>
+    </row>
+    <row r="5950" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5950" s="3">
+        <v>44301</v>
+      </c>
+      <c r="B5950" s="5">
+        <v>3665.49</v>
+      </c>
+    </row>
+    <row r="5951" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5951" s="4">
+        <v>44302</v>
+      </c>
+      <c r="B5951" s="6">
+        <v>3620.4</v>
+      </c>
+    </row>
+    <row r="5952" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5952" s="3">
+        <v>44303</v>
+      </c>
+      <c r="B5952" s="5">
+        <v>3595.57</v>
+      </c>
+    </row>
+    <row r="5953" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5953" s="4">
+        <v>44304</v>
+      </c>
+      <c r="B5953" s="6">
+        <v>3595.57</v>
+      </c>
+    </row>
+    <row r="5954" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5954" s="3">
+        <v>44305</v>
+      </c>
+      <c r="B5954" s="5">
+        <v>3595.57</v>
+      </c>
+    </row>
+    <row r="5955" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5955" s="4">
+        <v>44306</v>
+      </c>
+      <c r="B5955" s="6">
+        <v>3606.42</v>
+      </c>
+    </row>
+    <row r="5956" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5956" s="3">
+        <v>44307</v>
+      </c>
+      <c r="B5956" s="5">
+        <v>3636.26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>